<commit_message>
correcao use case add componente
</commit_message>
<xml_diff>
--- a/Use Cases.xlsx
+++ b/Use Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13800" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="EscolherJantes" sheetId="6" r:id="rId4"/>
     <sheet name="EscolherPneus" sheetId="7" r:id="rId5"/>
     <sheet name="EscolheDetalhesInteriores" sheetId="8" r:id="rId6"/>
-    <sheet name="VerificaCompatibilidade" sheetId="4" r:id="rId7"/>
+    <sheet name="AdicionaComponente" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
   <si>
     <t>Actor input</t>
   </si>
@@ -75,96 +75,7 @@
     <t>Cliente</t>
   </si>
   <si>
-    <t>1.Escolhe modelo do carro a configurar</t>
-  </si>
-  <si>
-    <t>2. Atualiza preço total da configuração</t>
-  </si>
-  <si>
     <t>Configuração ainda não foi inciada</t>
-  </si>
-  <si>
-    <t>Conflito entre componentes fica resolvido</t>
-  </si>
-  <si>
-    <t>Cenário  
-Alternativo
-[componentes incompatíveis]
-(passo 2)</t>
-  </si>
-  <si>
-    <t>2.1 Pergunta se deseja cancelar a seleção ou remover o componente incompatível</t>
-  </si>
-  <si>
-    <t>3. Adiciona componente à 
-configuração e atualiza o preço</t>
-  </si>
-  <si>
-    <t>1. Verifica se o item escolhido é incompatível com algum dos que já se 
-encontram na configuração</t>
-  </si>
-  <si>
-    <t>2. Confirma a seleção do componente
-caso não existam incompatibilidades</t>
-  </si>
-  <si>
-    <t>2.2 Escolhe manter a seleção</t>
-  </si>
-  <si>
-    <t>2.3 Elimina item incompativel
-Regressa a 3</t>
-  </si>
-  <si>
-    <t>Cenário  
-Alternativo
-[cancela a seleção]
-(passo 2.2)</t>
-  </si>
-  <si>
-    <r>
-      <t>Verificação de Compatibilidade(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Corpo)"/>
-      </rPr>
-      <t>mais que isso por ter atualizacao do preco ?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Corpo)"/>
-      </rPr>
-      <t>Sistema?Cliente?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -190,6 +101,67 @@
     </r>
   </si>
   <si>
+    <t>(tem?)</t>
+  </si>
+  <si>
+    <t>Escolher a pintura</t>
+  </si>
+  <si>
+    <t>Clliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escolher jantes </t>
+  </si>
+  <si>
+    <t>(só isto ? Adicionar mais coisas, cor das 
+jantes...?)</t>
+  </si>
+  <si>
+    <t>Escolher Pneus</t>
+  </si>
+  <si>
+    <t>Escolha detalhes interiores</t>
+  </si>
+  <si>
+    <t>(ex de um use case com mais detalhe)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Apresenta lista de materiais dos quais os estofos podem ser feitos
+</t>
+  </si>
+  <si>
+    <t>2. Escolhe o material desejado</t>
+  </si>
+  <si>
+    <t>3. Apresenta as cores existentes para 
+o material selecionado</t>
+  </si>
+  <si>
+    <t>4. Escolhe a cor pretendida</t>
+  </si>
+  <si>
+    <t>6. Apresenta lista de extras existentes</t>
+  </si>
+  <si>
+    <t>7. Seleciona os extras que deseja 
+aplicar</t>
+  </si>
+  <si>
+    <t>(E se não escolher uma cor ? Volta a 2? Mesmo para os extras, se não escolher nenhum?)</t>
+  </si>
+  <si>
+    <t>(adicionar cenario de excecao em que cliente não escolhe o modelo(?))</t>
+  </si>
+  <si>
+    <t>Modelo do carro já selecionado</t>
+  </si>
+  <si>
+    <t>Cor do carro é a escolhida pelo cliente e preço é atulizado</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <r>
       <t>(</t>
     </r>
@@ -199,7 +171,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Corpo)"/>
       </rPr>
-      <t>Sistema não faz nada.... Não tem de atualizar o preco nem nada...</t>
+      <t>Sistema?Cliente?Funcionario?</t>
     </r>
     <r>
       <rPr>
@@ -213,88 +185,171 @@
     </r>
   </si>
   <si>
-    <t>(tem?)</t>
-  </si>
-  <si>
-    <t>Escolher a pintura</t>
-  </si>
-  <si>
-    <t>Cor do carro é a escolhida pelo cliente (?)</t>
-  </si>
-  <si>
-    <t>1. Indica a cor pretendida</t>
-  </si>
-  <si>
-    <t>2.  Atualiza informação relativa à 
+    <t>3. Confirma a seleção do componente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Adiciona componente à
+configuração e atualiza o preço
+</t>
+  </si>
+  <si>
+    <t>Componente é adicionado e o preço atualizado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Verifica se o item escolhido obriga à instalação de outros componentes
+</t>
+  </si>
+  <si>
+    <t>1.1 Pergunta se deseja cancelar a seleção ou remover o componente incompatível</t>
+  </si>
+  <si>
+    <t>1.2 Escolhe manter a seleção</t>
+  </si>
+  <si>
+    <t>2.1 Pergunta se deseja instalar os componentes necessários</t>
+  </si>
+  <si>
+    <t>2.2 Aceita instalar os componentes</t>
+  </si>
+  <si>
+    <t>1.3 Elimina item incompativel e atualiza o preço
+Regressa a 2</t>
+  </si>
+  <si>
+    <t>2.3 Adiciona componentes à 
+configuração e atualiza o preço 
+Regressa a 3</t>
+  </si>
+  <si>
+    <t>Cenário  
+Alternativo 1
+[existem componentes incompatíveis]
+(passo 1)</t>
+  </si>
+  <si>
+    <t>Cenário  
+Alternativo 2
+[existem componentes complementares]
+(passo 2)</t>
+  </si>
+  <si>
+    <t>Cenário Excepção
+1  [cancela a seleção] (passo 1.2)</t>
+  </si>
+  <si>
+    <r>
+      <t>1.2.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Corpo)"/>
+      </rPr>
+      <t xml:space="preserve">(?) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corpo)"/>
+      </rPr>
+      <t>Recusa remover 
+componente incompatível</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.2 Informa que a seleção foi 
+cancelada </t>
+  </si>
+  <si>
+    <t>1. Verifica se o item escolhido é incompatível com algum dos que já se encontram na configuração</t>
+  </si>
+  <si>
+    <t>Cenário Excepção
+2  [cancela a seleção] (passo 2.2)</t>
+  </si>
+  <si>
+    <r>
+      <t>2.2.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Corpo)"/>
+      </rPr>
+      <t xml:space="preserve">(?) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corpo)"/>
+      </rPr>
+      <t>Recusa instalar 
+componentes necessários</t>
+    </r>
+  </si>
+  <si>
+    <t>2.2.2 Informa que a seleção foi
+ cancelada</t>
+  </si>
+  <si>
+    <t>(nas excepcoes as condicoes podem ser implicitras ?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adiciona Componente </t>
+  </si>
+  <si>
+    <t>5. &lt;&lt;include&gt;&gt; Adiciona Componente</t>
+  </si>
+  <si>
+    <t>8. &lt;&lt;include&gt;&gt; Adiciona Componente</t>
+  </si>
+  <si>
+    <t>1. Apresenta modelos existentes</t>
+  </si>
+  <si>
+    <t>2.Escolhe modelo do carro a
+ configurar</t>
+  </si>
+  <si>
+    <t>3.  Guarda opção e atualiza preço 
+total da configuração</t>
+  </si>
+  <si>
+    <t>1. Apresenta cores disponíveis</t>
+  </si>
+  <si>
+    <t>2. Indica a cor pretendida</t>
+  </si>
+  <si>
+    <t>3.  Atualiza informação relativa à 
 configuração e o respetivo preço</t>
   </si>
   <si>
-    <t>Clliente</t>
-  </si>
-  <si>
-    <t>1. Indica as jantes pretendidas</t>
-  </si>
-  <si>
-    <t>2. &lt;&lt;include&gt;&gt; VerificaCompatibilidade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Escolher jantes </t>
-  </si>
-  <si>
-    <t>(só isto ? Adicionar mais coisas, cor das 
-jantes...?)</t>
-  </si>
-  <si>
-    <t>Escolher Pneus</t>
-  </si>
-  <si>
-    <t>1. Indica penus pretendidos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Adicionar aqui o teste de complementaridade ?</t>
-  </si>
-  <si>
-    <t>Escolha detalhes interiores</t>
-  </si>
-  <si>
-    <t>(ex de um use case com mais detalhe)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Apresenta lista de materiais dos quais os estofos podem ser feitos
-</t>
-  </si>
-  <si>
-    <t>2. Escolhe o material desejado</t>
-  </si>
-  <si>
-    <t>3. Apresenta as cores existentes para 
-o material selecionado</t>
-  </si>
-  <si>
-    <t>4. Escolhe a cor pretendida</t>
-  </si>
-  <si>
-    <t>5. &lt;&lt;include&gt;&gt; VerificaCompatibilidade</t>
-  </si>
-  <si>
-    <t>6. Apresenta lista de extras existentes</t>
-  </si>
-  <si>
-    <t>7. Seleciona os extras que deseja 
-aplicar</t>
-  </si>
-  <si>
-    <t>8. &lt;&lt;include&gt;&gt; VerificaCompatibilidade</t>
-  </si>
-  <si>
-    <t>(E se não escolher uma cor ? Volta a 2? Mesmo para os extras, se não escolher nenhum?)</t>
+    <t>1. Apresenta jantes disponíveis</t>
+  </si>
+  <si>
+    <t>2. Indica as jantes pretendidas</t>
+  </si>
+  <si>
+    <t>3. &lt;&lt;include&gt;&gt; Adiciona Componente</t>
+  </si>
+  <si>
+    <t>1. Apresenta modelos de pneus
+ disponíveis</t>
+  </si>
+  <si>
+    <t>2. Indica pneus pretendidos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -319,6 +374,11 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri (Corpo)"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri (Corpo)"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -334,7 +394,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -477,11 +537,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -496,38 +600,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -537,6 +611,105 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -853,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -870,32 +1043,32 @@
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="19" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -906,73 +1079,73 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="14"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
     </row>
@@ -991,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D19"/>
+  <dimension ref="B1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:G10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1010,40 +1183,40 @@
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="12"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="12"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="12"/>
+      <c r="C4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="12"/>
+      <c r="C5" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="19" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1054,84 +1227,93 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
-      <c r="C7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="20"/>
+      <c r="C8" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="20"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="10" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="14"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="3"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="20"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="1"/>
+      <c r="C18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="3"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="16"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B18:B20"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B16"/>
-    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B6:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1139,7 +1321,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D19"/>
+  <dimension ref="B1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -1158,38 +1340,40 @@
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="12"/>
+      <c r="C2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="12"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
+      <c r="C4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="12"/>
+      <c r="C5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="19" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1200,84 +1384,91 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
-      <c r="C7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="20"/>
+      <c r="C8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="20"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="10" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="14"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="3"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="20"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="1"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="3"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="16"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B18:B20"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B16"/>
-    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B6:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1285,10 +1476,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D19"/>
+  <dimension ref="B1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1304,36 +1495,36 @@
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="12"/>
+      <c r="C2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="12"/>
+      <c r="C3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="19" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1344,86 +1535,93 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
-      <c r="C7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="1"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="15" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="20"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
+      <c r="D9" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="20"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="11" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="14"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="3"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="20"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="1"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="3"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="16"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B18:B20"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B16"/>
-    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B6:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1431,10 +1629,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D19"/>
+  <dimension ref="B1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1450,36 +1648,36 @@
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="12"/>
+      <c r="C2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="12"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="19" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1489,85 +1687,92 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
-      <c r="C7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="1"/>
+    <row r="7" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="19"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="43" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="14"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="3"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="20"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="1"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="3"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="16"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B18:B20"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B16"/>
-    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B6:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1577,8 +1782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1594,39 +1799,39 @@
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="12"/>
+      <c r="C2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="18"/>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="12"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="19" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1637,98 +1842,98 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="58" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="17" t="s">
-        <v>43</v>
+      <c r="D7" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="5" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="17" t="s">
-        <v>45</v>
+      <c r="D9" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="5" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="14"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
-      <c r="C13" s="23" t="s">
-        <v>49</v>
+      <c r="B13" s="20"/>
+      <c r="C13" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="24" t="s">
-        <v>51</v>
+      <c r="C17" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B17:B19"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="B6:B16"/>
-    <mergeCell ref="B17:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1736,188 +1941,205 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E24"/>
+  <dimension ref="B1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" customWidth="1"/>
-    <col min="4" max="4" width="37.5" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="66.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+    <row r="1" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+    </row>
+    <row r="2" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="22" t="s">
+      <c r="C2" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="27"/>
+      <c r="E2" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="27"/>
+    </row>
+    <row r="4" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="27"/>
+    </row>
+    <row r="5" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="27"/>
+    </row>
+    <row r="6" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="20"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="58" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="20"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="20"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="58" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="20"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="16"/>
+      <c r="C12" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="47"/>
+    </row>
+    <row r="13" spans="2:5" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="16"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="12"/>
-    </row>
-    <row r="6" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="58" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="14"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="2:4" ht="58" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10"/>
-      <c r="C18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="10"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="17"/>
-    </row>
-    <row r="22" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="10"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="17"/>
-    </row>
-    <row r="23" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="10"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="17"/>
-    </row>
-    <row r="24" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="10"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="3"/>
+    <row r="15" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="16"/>
+      <c r="C15" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="32"/>
+    </row>
+    <row r="16" spans="2:5" ht="58" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="16"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="16"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
+    </row>
+    <row r="18" spans="2:6" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="39"/>
+    </row>
+    <row r="19" spans="2:6" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="22"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="39"/>
+    </row>
+    <row r="21" spans="2:6" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="16"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="24"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B20:B24"/>
+  <mergeCells count="9">
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B16"/>
-    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
uses cases: motorização e gestao fabrica
</commit_message>
<xml_diff>
--- a/Use Cases.xlsx
+++ b/Use Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Documents\MIEI\3º Ano\1º Semestre\Desenvolvimento de Sistemas de Software\Projeto\dss-projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\MIEI\3º Ano\1º Semestre\Desenvolvimento de Sistemas de Software\Projeto\dss-projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A549B629-73B6-4719-9356-4183677D5CCD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3820037-9C3C-4117-BD00-67DF7DDF4150}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="13800" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="13800" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,11 @@
     <sheet name="EscolhePintura" sheetId="5" r:id="rId3"/>
     <sheet name="EscolherJantes" sheetId="6" r:id="rId4"/>
     <sheet name="EscolherPneus" sheetId="7" r:id="rId5"/>
-    <sheet name="EscolheDetalhesInteriores" sheetId="8" r:id="rId6"/>
-    <sheet name="AdicionaComponente" sheetId="4" r:id="rId7"/>
+    <sheet name="EscolherMotorização" sheetId="9" r:id="rId6"/>
+    <sheet name="EscolheDetalhesInteriores" sheetId="8" r:id="rId7"/>
+    <sheet name="AdicionaComponente" sheetId="4" r:id="rId8"/>
+    <sheet name="RegistarEntradaStock" sheetId="10" r:id="rId9"/>
+    <sheet name="EncomendarStock" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="101">
   <si>
     <t>Actor input</t>
   </si>
@@ -351,12 +354,120 @@
   <si>
     <t>2.4 Regressa a 3</t>
   </si>
+  <si>
+    <t>1. Apresenta motorizações disponíveis</t>
+  </si>
+  <si>
+    <t>2. Indica a motorização pretendida</t>
+  </si>
+  <si>
+    <t>Pneus do carro já selecionados</t>
+  </si>
+  <si>
+    <t>Motorização é a escolhida pelo cliente e preço é atualizado</t>
+  </si>
+  <si>
+    <t>Escolher Motorização</t>
+  </si>
+  <si>
+    <t>3.  &lt;&lt;include&gt;&gt; Adiciona Componente</t>
+  </si>
+  <si>
+    <t>Registar Entrada de Stock</t>
+  </si>
+  <si>
+    <t>Gestor de Fábrica</t>
+  </si>
+  <si>
+    <t>Stock de cada componente é atualizado</t>
+  </si>
+  <si>
+    <t>1. Apresenta componentes e o seu stock</t>
+  </si>
+  <si>
+    <t>2. Indica para cada componente 
+qual o stock que chegou</t>
+  </si>
+  <si>
+    <t>3. Atualiza e regista o stock atual de cada componente</t>
+  </si>
+  <si>
+    <t>4. Indica quais os carros que podem 
+ser produzidos ???</t>
+  </si>
+  <si>
+    <t>1.1. Adiciona componente ao sistema 
+e adiciona o seu stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2. Regista novo componente e atualiza 
+o seu stock </t>
+  </si>
+  <si>
+    <t>Cenário Exceção 1
+[componente não existente no sistema]
+(passo 2)</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Encomendar Stock</t>
+  </si>
+  <si>
+    <t>Existem componentes com stock igual a 0</t>
+  </si>
+  <si>
+    <t>2. Indica quais os componentes que pretende encomendar e a sua quantidade</t>
+  </si>
+  <si>
+    <t>3. Encomenda componentes e quantidades indicadas aos fornecedores</t>
+  </si>
+  <si>
+    <t>Cenário Exceção 1
+[não indica componentes]
+(passo 2)</t>
+  </si>
+  <si>
+    <t>1.1. Não indica os componentes</t>
+  </si>
+  <si>
+    <t>1.2. Informa que seleção foi cancelada</t>
+  </si>
+  <si>
+    <t>Cenário Exceção 2
+[não indica quantidades]
+(passo 2)</t>
+  </si>
+  <si>
+    <t>2.1. Não indica as quantidades</t>
+  </si>
+  <si>
+    <t>2.2. Informa que seleção foi cancelada</t>
+  </si>
+  <si>
+    <t>Cenário Exceção  3
+[componente não existente no sistema]
+(passo 2)</t>
+  </si>
+  <si>
+    <t>3.1. Indica que componente não existe no sistema</t>
+  </si>
+  <si>
+    <t>3.3. Adiciona novo componente ao 
+sistema e adiciona-o à lista de 
+componentes a encomendar</t>
+  </si>
+  <si>
+    <t>3.2. Indica novo componente a 
+encomendar e a sua quantidade</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -393,6 +504,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -599,7 +729,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -691,6 +821,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -724,7 +855,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1058,32 +1208,32 @@
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="41" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1094,73 +1244,73 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B7" s="41"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B8" s="41"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B9" s="41"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B10" s="41"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B11" s="41"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B12" s="41"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B13" s="41"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B14" s="41"/>
+      <c r="B14" s="42"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B15" s="41"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B16" s="41"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="38" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B18" s="37"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B19" s="37"/>
+      <c r="B19" s="38"/>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
     </row>
@@ -1174,6 +1324,176 @@
     <mergeCell ref="B6:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F3ED6C-B1F6-4EC6-94BA-9047DB90E28E}">
+  <dimension ref="B1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="15.375" customWidth="1"/>
+    <col min="3" max="3" width="36.75" customWidth="1"/>
+    <col min="4" max="4" width="40.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="2" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="40"/>
+    </row>
+    <row r="3" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="40"/>
+    </row>
+    <row r="4" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="40"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="40"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B6" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B7" s="41"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="57" thickBot="1">
+      <c r="B8" s="42"/>
+      <c r="C8" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="55"/>
+    </row>
+    <row r="9" spans="2:4" ht="57" thickBot="1">
+      <c r="B9" s="42"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B10" s="42"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="50"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B11" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B12" s="38"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="58.5" customHeight="1" thickBot="1">
+      <c r="B13" s="38"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B14" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B15" s="38"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="60.75" customHeight="1" thickBot="1">
+      <c r="B16" s="38"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B17" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B18" s="38"/>
+      <c r="C18" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="2:4" ht="58.5" customHeight="1" thickBot="1">
+      <c r="B19" s="38"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="56" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B11:B13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1198,40 +1518,40 @@
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="39"/>
+      <c r="D2" s="40"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="39"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="39"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="41" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1242,68 +1562,68 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B7" s="40"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="31"/>
       <c r="D7" s="15" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B8" s="41"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B9" s="41"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="5"/>
       <c r="D9" s="10" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B10" s="41"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B11" s="41"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B12" s="41"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B13" s="41"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B14" s="41"/>
+      <c r="B14" s="42"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B15" s="41"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B16" s="41"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B17" s="41"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="38" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="14" t="s">
@@ -1312,12 +1632,12 @@
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B19" s="37"/>
+      <c r="B19" s="38"/>
       <c r="C19" s="5"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B20" s="37"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="6"/>
       <c r="D20" s="3"/>
     </row>
@@ -1339,7 +1659,7 @@
   <dimension ref="B1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1355,40 +1675,40 @@
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="39"/>
+      <c r="D2" s="40"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="39"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="39"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="41" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1399,45 +1719,45 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B7" s="40"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="31"/>
       <c r="D7" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B8" s="41"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B9" s="41"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="5"/>
       <c r="D9" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B10" s="41"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="38" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B12" s="37"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B13" s="37"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="6"/>
       <c r="D13" s="3"/>
     </row>
@@ -1458,7 +1778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1475,36 +1795,36 @@
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="39"/>
+      <c r="D2" s="40"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="39"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="41" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1515,82 +1835,82 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B7" s="40"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="31"/>
       <c r="D7" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B8" s="41"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B9" s="41"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="55.5" thickBot="1">
-      <c r="B10" s="41"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="5"/>
       <c r="D10" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B11" s="41"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B12" s="41"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B13" s="41"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B14" s="41"/>
+      <c r="B14" s="42"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B15" s="41"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B16" s="41"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B17" s="41"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="38" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B19" s="37"/>
+      <c r="B19" s="38"/>
       <c r="C19" s="5"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B20" s="37"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="6"/>
       <c r="D20" s="3"/>
     </row>
@@ -1611,7 +1931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1628,36 +1948,36 @@
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="39"/>
+      <c r="D2" s="40"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="39"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="41" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1668,80 +1988,80 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B7" s="40"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="31"/>
       <c r="D7" s="32" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B8" s="41"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="5" t="s">
         <v>65</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B9" s="41"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B10" s="41"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B11" s="41"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B12" s="41"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B13" s="41"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B14" s="41"/>
+      <c r="B14" s="42"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B15" s="41"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B16" s="41"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B17" s="41"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="38" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B19" s="37"/>
+      <c r="B19" s="38"/>
       <c r="C19" s="5"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B20" s="37"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="6"/>
       <c r="D20" s="3"/>
     </row>
@@ -1759,11 +2079,131 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3EA4158-361D-48CA-9195-2D172A413870}">
+  <dimension ref="B1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="16.75" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="35.75" customWidth="1"/>
+    <col min="4" max="4" width="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="2" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="40"/>
+    </row>
+    <row r="3" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="40"/>
+    </row>
+    <row r="4" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="40"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="40"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B6" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B7" s="41"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B8" s="42"/>
+      <c r="C8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B9" s="42"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B10" s="42"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B11" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B12" s="38"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B13" s="38"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B11:B13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1779,10 +2219,10 @@
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" t="s">
         <v>21</v>
       </c>
@@ -1791,27 +2231,27 @@
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="39"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="2:5" ht="19.5" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="41" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1822,73 +2262,73 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="57" thickBot="1">
-      <c r="B7" s="41"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="5"/>
       <c r="D7" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B8" s="41"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:5" ht="38.25" thickBot="1">
-      <c r="B9" s="41"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="5"/>
       <c r="D9" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B10" s="41"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B11" s="41"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B12" s="41"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="38.25" thickBot="1">
-      <c r="B13" s="41"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="13" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B14" s="41"/>
+      <c r="B14" s="42"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B15" s="41"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B16" s="41"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="38" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="14" t="s">
@@ -1897,12 +2337,12 @@
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B18" s="37"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B19" s="37"/>
+      <c r="B19" s="38"/>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
     </row>
@@ -1919,11 +2359,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -1944,10 +2384,10 @@
       <c r="B2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="12" t="s">
         <v>31</v>
       </c>
@@ -1956,31 +2396,31 @@
       <c r="B3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="46"/>
+      <c r="D3" s="47"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" thickBot="1">
       <c r="B4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="46"/>
+      <c r="D4" s="47"/>
     </row>
     <row r="5" spans="2:5" ht="19.5" thickBot="1">
       <c r="B5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="46"/>
+      <c r="D5" s="47"/>
     </row>
     <row r="6" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="41" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -1991,35 +2431,35 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="71.099999999999994" customHeight="1" thickBot="1">
-      <c r="B7" s="41"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="20"/>
       <c r="D7" s="21" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="57" thickBot="1">
-      <c r="B8" s="41"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="20"/>
       <c r="D8" s="21" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B9" s="41"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="20"/>
       <c r="D9" s="21" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="57" thickBot="1">
-      <c r="B10" s="41"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="20"/>
       <c r="D10" s="21" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="38.25" thickBot="1">
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="44" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="22"/>
@@ -2028,21 +2468,21 @@
       </c>
     </row>
     <row r="12" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B12" s="37"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="34" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="36"/>
     </row>
     <row r="13" spans="2:5" ht="38.25" thickBot="1">
-      <c r="B13" s="37"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="33"/>
       <c r="D13" s="35" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="45" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="20"/>
@@ -2051,28 +2491,28 @@
       </c>
     </row>
     <row r="15" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B15" s="37"/>
+      <c r="B15" s="38"/>
       <c r="C15" s="20" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="21"/>
     </row>
     <row r="16" spans="2:5" ht="57" thickBot="1">
-      <c r="B16" s="37"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="20"/>
       <c r="D16" s="21" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="19.5" thickBot="1">
-      <c r="B17" s="37"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="24"/>
       <c r="D17" s="25" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="44" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="27" t="s">
@@ -2081,14 +2521,14 @@
       <c r="D18" s="28"/>
     </row>
     <row r="19" spans="2:6" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="B19" s="43"/>
+      <c r="B19" s="44"/>
       <c r="C19" s="29"/>
       <c r="D19" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="38.1" customHeight="1" thickBot="1">
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="44" t="s">
         <v>48</v>
       </c>
       <c r="C20" s="27" t="s">
@@ -2097,7 +2537,7 @@
       <c r="D20" s="28"/>
     </row>
     <row r="21" spans="2:6" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="B21" s="37"/>
+      <c r="B21" s="38"/>
       <c r="C21" s="24"/>
       <c r="D21" s="26" t="s">
         <v>50</v>
@@ -2112,7 +2552,7 @@
       <c r="D22" s="16"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="37" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2131,4 +2571,131 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABD9931-D77D-426A-864E-2D03D3F76F86}">
+  <dimension ref="B1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="15.375" customWidth="1"/>
+    <col min="3" max="3" width="36.75" customWidth="1"/>
+    <col min="4" max="4" width="40.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="16.5" thickBot="1"/>
+    <row r="2" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="40"/>
+    </row>
+    <row r="3" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="40"/>
+    </row>
+    <row r="4" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="40"/>
+    </row>
+    <row r="5" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="40"/>
+    </row>
+    <row r="6" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B6" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B7" s="41"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="53"/>
+    </row>
+    <row r="8" spans="2:5" ht="38.25" thickBot="1">
+      <c r="B8" s="42"/>
+      <c r="C8" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:5" ht="38.25" thickBot="1">
+      <c r="B9" s="42"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="38.25" thickBot="1">
+      <c r="B10" s="42"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="50" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="57" thickBot="1">
+      <c r="B11" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="2:5" ht="56.25" customHeight="1" thickBot="1">
+      <c r="B12" s="38"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="19.5" customHeight="1" thickBot="1">
+      <c r="B13" s="38"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B11:B13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionado os uses cases da gestão de cliente
</commit_message>
<xml_diff>
--- a/Use Cases.xlsx
+++ b/Use Cases.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27610"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Documents\MIEI\3º Ano\1º Semestre\Desenvolvimento de Sistemas de Software\Projeto\dss-projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ambrosiny/Desktop/Universidade/3ano/DSS/Trabalho_DSS/dss-projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AA13E9-696D-4581-9CD8-AA5B1D6B7315}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="13800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13000" yWindow="0" windowWidth="12600" windowHeight="16000" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,24 +17,27 @@
     <sheet name="Registar Entrada Stock" sheetId="10" r:id="rId3"/>
     <sheet name="Encomendar Stock" sheetId="11" r:id="rId4"/>
     <sheet name="Adiciona Pacote" sheetId="12" r:id="rId5"/>
+    <sheet name="Consultar cliente" sheetId="13" r:id="rId6"/>
+    <sheet name="Registar cliente" sheetId="14" r:id="rId7"/>
+    <sheet name="Alterar Cliente" sheetId="15" r:id="rId8"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="117">
   <si>
     <t>Actor input</t>
   </si>
@@ -354,12 +356,124 @@
   <si>
     <t>2.3. Regressa a 3</t>
   </si>
+  <si>
+    <t>Consultar cliente</t>
+  </si>
+  <si>
+    <t>Funcionário autenticado</t>
+  </si>
+  <si>
+    <t>Dados do cliente consultados</t>
+  </si>
+  <si>
+    <t>1. Indica o cliente 
+que pretende consultar</t>
+  </si>
+  <si>
+    <t>2. Verifica se o cliente existe</t>
+  </si>
+  <si>
+    <t>3. Mostra os dados do mesmo</t>
+  </si>
+  <si>
+    <t>Cenário Excepção 1 
+[Cliente não existe] 
+(Passo 2)</t>
+  </si>
+  <si>
+    <t>2.1 Informa que o cliente não existe</t>
+  </si>
+  <si>
+    <t>4. Consulta os dados</t>
+  </si>
+  <si>
+    <t>Alterar Cliente</t>
+  </si>
+  <si>
+    <t>1. Indica o cliente 
+que pretende alterar</t>
+  </si>
+  <si>
+    <t>Ficha do cliente atualizado</t>
+  </si>
+  <si>
+    <t>3. Mostra a ficha do cliente</t>
+  </si>
+  <si>
+    <t>5. Regista as alterações no sistema</t>
+  </si>
+  <si>
+    <t>Cenário Excepção 1 
+[Cliente não existe] 
+(passo 2)</t>
+  </si>
+  <si>
+    <t>4. Indica os campos a alterar
+ e as respetivas alterações</t>
+  </si>
+  <si>
+    <t>4.1 Indica que não quer 
+fazer alterações</t>
+  </si>
+  <si>
+    <t>4.2 Informa que o cliente
+ permaneceu inalterado</t>
+  </si>
+  <si>
+    <t>Cenário Excepção 2 
+[Nenhuma alteração] 
+(passo 4)</t>
+  </si>
+  <si>
+    <t>Registar Cliente</t>
+  </si>
+  <si>
+    <t>Funcionário Autenticado</t>
+  </si>
+  <si>
+    <t>Cliente adicionado à base de dados</t>
+  </si>
+  <si>
+    <t>1. Indica o cliente
+ que vai ser adicionado</t>
+  </si>
+  <si>
+    <t>2. Verifica se o cliente já existe</t>
+  </si>
+  <si>
+    <t>3. Mostra os campos 
+com os dados a preencher</t>
+  </si>
+  <si>
+    <t>4. Preenche os dados 
+do novo cliente</t>
+  </si>
+  <si>
+    <t>5. Adiciona o cliente</t>
+  </si>
+  <si>
+    <t>Cenário Exepção 1 
+[Cliente já existe] 
+(Passo 2)</t>
+  </si>
+  <si>
+    <t>2.1 Informa que o cliente já existe</t>
+  </si>
+  <si>
+    <t>Cenário Exepção 2 
+[Campos por preencher] 
+(Passo 4)</t>
+  </si>
+  <si>
+    <t>4.1 Informa que o cliente 
+não pode ser adicionado</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -397,6 +511,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Corpo)"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri (Corpo)"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -412,7 +536,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -625,11 +749,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -721,6 +860,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -736,6 +905,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -751,50 +926,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1109,52 +1265,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="16.125" customWidth="1"/>
-    <col min="3" max="3" width="33.375" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
     <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="16.5" thickBot="1"/>
-    <row r="2" spans="2:4" ht="19.5" thickBot="1">
+    <row r="1" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39"/>
-    </row>
-    <row r="3" spans="2:4" ht="19.5" thickBot="1">
+      <c r="C2" s="48"/>
+      <c r="D2" s="49"/>
+    </row>
+    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39"/>
-    </row>
-    <row r="4" spans="2:4" ht="19.5" thickBot="1">
+      <c r="C3" s="48"/>
+      <c r="D3" s="49"/>
+    </row>
+    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" thickBot="1">
+      <c r="C4" s="48"/>
+      <c r="D4" s="49"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B6" s="40" t="s">
+      <c r="C5" s="48"/>
+      <c r="D5" s="49"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="50" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1164,74 +1320,74 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B7" s="41"/>
+    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="51"/>
       <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B8" s="41"/>
+    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="51"/>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B9" s="41"/>
+    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="51"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B10" s="41"/>
+    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="51"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B11" s="41"/>
+    <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="51"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B12" s="41"/>
+    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="51"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B13" s="41"/>
+    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="51"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B14" s="41"/>
+    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="51"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B15" s="41"/>
+    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="51"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B16" s="41"/>
+    <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="51"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B17" s="37" t="s">
+    <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="47" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B18" s="37"/>
+    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="47"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B19" s="37"/>
+    <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="47"/>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
     </row>
@@ -1249,67 +1405,67 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="B23" sqref="B23:D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="23.875" customWidth="1"/>
-    <col min="3" max="3" width="40.625" customWidth="1"/>
-    <col min="4" max="4" width="66.625" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="66.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="16.5" thickBot="1">
+    <row r="1" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
     </row>
-    <row r="2" spans="2:5" ht="19.5" thickBot="1">
+    <row r="2" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="45"/>
+      <c r="D2" s="57"/>
       <c r="E2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="19.5" thickBot="1">
+    <row r="3" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="45"/>
-    </row>
-    <row r="4" spans="2:5" ht="19.5" thickBot="1">
+      <c r="D3" s="57"/>
+    </row>
+    <row r="4" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="45"/>
-    </row>
-    <row r="5" spans="2:5" ht="19.5" thickBot="1">
+      <c r="D4" s="57"/>
+    </row>
+    <row r="5" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="45"/>
-    </row>
-    <row r="6" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B6" s="40" t="s">
+      <c r="D5" s="57"/>
+    </row>
+    <row r="6" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="50" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -1319,50 +1475,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B7" s="40"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51" t="s">
+    <row r="7" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="50"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="39" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B8" s="40"/>
-      <c r="C8" s="52" t="s">
+    <row r="8" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="50"/>
+      <c r="C8" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="49"/>
-    </row>
-    <row r="9" spans="2:5" ht="71.099999999999994" customHeight="1" thickBot="1">
-      <c r="B9" s="41"/>
+      <c r="D8" s="37"/>
+    </row>
+    <row r="9" spans="2:5" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="51"/>
       <c r="C9" s="18"/>
       <c r="D9" s="19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="57" thickBot="1">
-      <c r="B10" s="41"/>
+    <row r="10" spans="2:5" ht="58" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="51"/>
       <c r="C10" s="18"/>
       <c r="D10" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B11" s="41"/>
+    <row r="11" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="51"/>
       <c r="C11" s="18"/>
       <c r="D11" s="19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="57" thickBot="1">
-      <c r="B12" s="41"/>
+    <row r="12" spans="2:5" ht="58" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="51"/>
       <c r="C12" s="18"/>
       <c r="D12" s="19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="38.25" thickBot="1">
-      <c r="B13" s="42" t="s">
+    <row r="13" spans="2:5" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="54" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="20"/>
@@ -1370,22 +1526,22 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B14" s="37"/>
+    <row r="14" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="47"/>
       <c r="C14" s="29" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="31"/>
     </row>
-    <row r="15" spans="2:5" ht="39.75" customHeight="1" thickBot="1">
-      <c r="B15" s="37"/>
+    <row r="15" spans="2:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="47"/>
       <c r="C15" s="28"/>
       <c r="D15" s="30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="19.5" thickBot="1">
-      <c r="B16" s="43" t="s">
+    <row r="16" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="55" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="18"/>
@@ -1393,22 +1549,22 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="19.5" thickBot="1">
-      <c r="B17" s="37"/>
+    <row r="17" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="47"/>
       <c r="C17" s="18" t="s">
         <v>39</v>
       </c>
       <c r="D17" s="19"/>
     </row>
-    <row r="18" spans="2:6" ht="51.75" customHeight="1" thickBot="1">
-      <c r="B18" s="37"/>
+    <row r="18" spans="2:6" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="47"/>
       <c r="C18" s="22"/>
       <c r="D18" s="23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="39.950000000000003" customHeight="1">
-      <c r="B19" s="53" t="s">
+    <row r="19" spans="2:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="52" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="25" t="s">
@@ -1416,15 +1572,15 @@
       </c>
       <c r="D19" s="26"/>
     </row>
-    <row r="20" spans="2:6" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="B20" s="54"/>
+    <row r="20" spans="2:6" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="53"/>
       <c r="C20" s="27"/>
       <c r="D20" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="38.1" customHeight="1" thickBot="1">
-      <c r="B21" s="42" t="s">
+    <row r="21" spans="2:6" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="54" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="25" t="s">
@@ -1432,16 +1588,16 @@
       </c>
       <c r="D21" s="26"/>
     </row>
-    <row r="22" spans="2:6" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="B22" s="37"/>
+    <row r="22" spans="2:6" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="47"/>
       <c r="C22" s="22"/>
       <c r="D22" s="24" t="s">
         <v>48</v>
       </c>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="2:6" ht="18.75">
-      <c r="B23" s="53" t="s">
+    <row r="23" spans="2:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="B23" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C23" s="25" t="s">
@@ -1449,9 +1605,9 @@
       </c>
       <c r="D23" s="26"/>
     </row>
-    <row r="24" spans="2:6" ht="47.25" customHeight="1" thickBot="1">
-      <c r="B24" s="54"/>
-      <c r="C24" s="55"/>
+    <row r="24" spans="2:6" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="53"/>
+      <c r="C24" s="41"/>
       <c r="D24" s="24" t="s">
         <v>51</v>
       </c>
@@ -1475,59 +1631,59 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABD9931-D77D-426A-864E-2D03D3F76F86}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.375" customWidth="1"/>
-    <col min="3" max="3" width="36.75" customWidth="1"/>
-    <col min="4" max="4" width="40.125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="40.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="16.5" thickBot="1"/>
-    <row r="2" spans="2:4" ht="19.5" thickBot="1">
+    <row r="1" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="39"/>
-    </row>
-    <row r="3" spans="2:4" ht="19.5" thickBot="1">
+      <c r="D2" s="49"/>
+    </row>
+    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="39"/>
-    </row>
-    <row r="4" spans="2:4" ht="19.5" thickBot="1">
+      <c r="D3" s="49"/>
+    </row>
+    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="58"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" thickBot="1">
+      <c r="D4" s="60"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="39"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B6" s="40" t="s">
+      <c r="D5" s="49"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="50" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1537,52 +1693,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B7" s="41"/>
+    <row r="7" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="51"/>
       <c r="C7" s="12" t="s">
         <v>80</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B8" s="41"/>
+    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="51"/>
       <c r="C8" s="12"/>
       <c r="D8" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B9" s="41"/>
+    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="51"/>
       <c r="C9" s="12" t="s">
         <v>81</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B10" s="41"/>
+    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="51"/>
       <c r="C10" s="5"/>
       <c r="D10" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="38.25" customHeight="1" thickBot="1">
-      <c r="B11" s="42" t="s">
+    <row r="11" spans="2:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="44" t="s">
         <v>83</v>
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" ht="38.25" customHeight="1" thickBot="1">
-      <c r="B12" s="42"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="61" t="s">
+    <row r="12" spans="2:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="54"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="46" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="56.25" customHeight="1" thickBot="1">
-      <c r="B13" s="37"/>
+    <row r="13" spans="2:4" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="47"/>
       <c r="C13" s="6"/>
       <c r="D13" s="24" t="s">
         <v>85</v>
@@ -1603,55 +1759,55 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F3ED6C-B1F6-4EC6-94BA-9047DB90E28E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.375" customWidth="1"/>
-    <col min="3" max="3" width="36.75" customWidth="1"/>
-    <col min="4" max="4" width="40.125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="40.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="16.5" thickBot="1"/>
-    <row r="2" spans="2:4" ht="19.5" thickBot="1">
+    <row r="1" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="39"/>
-    </row>
-    <row r="3" spans="2:4" ht="19.5" thickBot="1">
+      <c r="D2" s="49"/>
+    </row>
+    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="39"/>
-    </row>
-    <row r="4" spans="2:4" ht="19.5" thickBot="1">
+      <c r="D3" s="49"/>
+    </row>
+    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="39"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" thickBot="1">
+      <c r="C4" s="59"/>
+      <c r="D4" s="49"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="39"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B6" s="40" t="s">
+      <c r="C5" s="61"/>
+      <c r="D5" s="49"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="50" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1661,34 +1817,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B7" s="40"/>
+    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="50"/>
       <c r="C7" s="32"/>
       <c r="D7" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="57" thickBot="1">
-      <c r="B8" s="41"/>
+    <row r="8" spans="2:4" ht="58" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="51"/>
       <c r="C8" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="35"/>
     </row>
-    <row r="9" spans="2:4" ht="57" thickBot="1">
-      <c r="B9" s="41"/>
+    <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="51"/>
       <c r="C9" s="5"/>
       <c r="D9" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B10" s="41"/>
+    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="51"/>
       <c r="C10" s="5"/>
       <c r="D10" s="33"/>
     </row>
-    <row r="11" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B11" s="42" t="s">
+    <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="54" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="34" t="s">
@@ -1696,20 +1852,20 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B12" s="37"/>
+    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="47"/>
       <c r="C12" s="5"/>
       <c r="D12" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="58.5" customHeight="1" thickBot="1">
-      <c r="B13" s="37"/>
+    <row r="13" spans="2:4" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="47"/>
       <c r="C13" s="6"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B14" s="42" t="s">
+    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="54" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="34" t="s">
@@ -1717,20 +1873,20 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B15" s="37"/>
+    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="47"/>
       <c r="C15" s="5"/>
       <c r="D15" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="60.75" customHeight="1" thickBot="1">
-      <c r="B16" s="37"/>
+    <row r="16" spans="2:4" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="47"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B17" s="42" t="s">
+    <row r="17" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="54" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="34" t="s">
@@ -1738,15 +1894,15 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B18" s="37"/>
+    <row r="18" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="47"/>
       <c r="C18" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="2:4" ht="58.5" customHeight="1" thickBot="1">
-      <c r="B19" s="37"/>
+    <row r="19" spans="2:4" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="47"/>
       <c r="C19" s="6"/>
       <c r="D19" s="36" t="s">
         <v>26</v>
@@ -1769,60 +1925,60 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90AC7C44-14F4-481B-9C40-B98399113727}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="18.75" customWidth="1"/>
-    <col min="3" max="3" width="33.375" customWidth="1"/>
-    <col min="4" max="4" width="53.375" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="16.5" thickBot="1"/>
-    <row r="2" spans="2:4" ht="19.5" thickBot="1">
+    <row r="1" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="39"/>
-    </row>
-    <row r="3" spans="2:4" ht="19.5" thickBot="1">
+      <c r="D2" s="49"/>
+    </row>
+    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="39"/>
-    </row>
-    <row r="4" spans="2:4" ht="19.5" thickBot="1">
+      <c r="D3" s="49"/>
+    </row>
+    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="39"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" thickBot="1">
+      <c r="D4" s="49"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="39"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B6" s="40" t="s">
+      <c r="D5" s="49"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="50" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1832,68 +1988,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B7" s="41"/>
+    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="51"/>
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B8" s="41"/>
+    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="51"/>
       <c r="C8" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B9" s="41"/>
+    <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="51"/>
       <c r="C9" s="5"/>
       <c r="D9" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B10" s="41"/>
+    <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="51"/>
       <c r="C10" s="5"/>
       <c r="D10" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B11" s="41"/>
+    <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="51"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="57" t="s">
+      <c r="D11" s="43" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B12" s="41"/>
+    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="51"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B13" s="41"/>
+    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="51"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B14" s="41"/>
+    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="51"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B15" s="41"/>
+    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="51"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B16" s="41"/>
+    <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="51"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B17" s="42" t="s">
+    <row r="17" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="54" t="s">
         <v>59</v>
       </c>
       <c r="C17" s="4"/>
@@ -1901,73 +2057,73 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B18" s="37"/>
+    <row r="18" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="47"/>
       <c r="C18" s="12" t="s">
         <v>62</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B19" s="37"/>
+    <row r="19" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="47"/>
       <c r="C19" s="12"/>
       <c r="D19" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B20" s="37"/>
+    <row r="20" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="47"/>
       <c r="C20" s="12"/>
       <c r="D20" s="19" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="24" customHeight="1" thickBot="1">
-      <c r="B21" s="37"/>
+    <row r="21" spans="2:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="47"/>
       <c r="C21" s="6"/>
       <c r="D21" s="23" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B22" s="42" t="s">
+    <row r="22" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="54" t="s">
         <v>60</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="56" t="s">
+      <c r="D22" s="42" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B23" s="37"/>
+    <row r="23" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="47"/>
       <c r="C23" s="12" t="s">
         <v>65</v>
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B24" s="37"/>
+    <row r="24" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="47"/>
       <c r="C24" s="12"/>
       <c r="D24" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="38.25" thickBot="1">
-      <c r="B25" s="37"/>
+    <row r="25" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="47"/>
       <c r="C25" s="12"/>
       <c r="D25" s="19" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B26" s="37"/>
+    <row r="26" spans="2:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="47"/>
       <c r="C26" s="6"/>
       <c r="D26" s="23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="18.75">
-      <c r="B27" s="53" t="s">
+    <row r="27" spans="2:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="B27" s="52" t="s">
         <v>74</v>
       </c>
       <c r="C27" s="25" t="s">
@@ -1975,9 +2131,9 @@
       </c>
       <c r="D27" s="26"/>
     </row>
-    <row r="28" spans="2:4" ht="54" customHeight="1" thickBot="1">
-      <c r="B28" s="54"/>
-      <c r="C28" s="55"/>
+    <row r="28" spans="2:4" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="53"/>
+      <c r="C28" s="41"/>
       <c r="D28" s="24" t="s">
         <v>73</v>
       </c>
@@ -1995,4 +2151,462 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:E16"/>
+  <sheetViews>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
+    <col min="5" max="5" width="37.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="49"/>
+    </row>
+    <row r="6" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="49"/>
+    </row>
+    <row r="7" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="49"/>
+    </row>
+    <row r="8" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="49"/>
+    </row>
+    <row r="9" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="51"/>
+      <c r="D10" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="51"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="51"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="51"/>
+      <c r="D13" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="51"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="51"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="3:5" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="64"/>
+      <c r="E16" s="65" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C9:C15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:D24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D27" sqref="D25:D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.5" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="49"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="49"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="49"/>
+    </row>
+    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="49"/>
+    </row>
+    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="51"/>
+      <c r="C9" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="51"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="51"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="51"/>
+      <c r="C12" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="51"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="51"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="51"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="51"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="51"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="51"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="47"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="47"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="62" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="42" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="47"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="47"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B8:B18"/>
+    <mergeCell ref="B19:B21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:D21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="49"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="49"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="49"/>
+    </row>
+    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="49"/>
+    </row>
+    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="51"/>
+      <c r="C9" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="51"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="51"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="51"/>
+      <c r="C12" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="51"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="51"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="51"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="51"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="51"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="51"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="2:4" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="64"/>
+      <c r="D19" s="65" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="47"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B8:B18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
uc encomendar + interface funcionario + relatorio up
</commit_message>
<xml_diff>
--- a/Use Cases.xlsx
+++ b/Use Cases.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27610"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ambrosiny/Desktop/Universidade/3ano/DSS/Trabalho_DSS/dss-projeto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\MIEI\3º Ano\1º Semestre\Desenvolvimento de Sistemas de Software\Projeto\dss-projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90F2E65-7603-41CD-BF4D-4303E53A2F24}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14060" yWindow="0" windowWidth="11540" windowHeight="16000" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="14055" yWindow="0" windowWidth="11535" windowHeight="16005" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,18 +29,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="137">
   <si>
     <t>Actor input</t>
   </si>
@@ -84,16 +85,7 @@
     <t>Gestor de Fábrica</t>
   </si>
   <si>
-    <t>1. Apresenta componentes e o seu stock</t>
-  </si>
-  <si>
     <t>Encomendar Stock</t>
-  </si>
-  <si>
-    <t>2. Indica quais os componentes que pretende encomendar e a sua quantidade</t>
-  </si>
-  <si>
-    <t>3. Encomenda componentes e quantidades indicadas aos fornecedores</t>
   </si>
   <si>
     <t>Cenário Exceção 1
@@ -101,38 +93,7 @@
 (passo 2)</t>
   </si>
   <si>
-    <t>1.1. Não indica os componentes</t>
-  </si>
-  <si>
-    <t>1.2. Informa que seleção foi cancelada</t>
-  </si>
-  <si>
-    <t>Cenário Exceção 2
-[não indica quantidades]
-(passo 2)</t>
-  </si>
-  <si>
-    <t>2.1. Não indica as quantidades</t>
-  </si>
-  <si>
     <t>2.2. Informa que seleção foi cancelada</t>
-  </si>
-  <si>
-    <t>Cenário Exceção  3
-[componente não existente no sistema]
-(passo 2)</t>
-  </si>
-  <si>
-    <t>3.1. Indica que componente não existe no sistema</t>
-  </si>
-  <si>
-    <t>3.3. Adiciona novo componente ao 
-sistema e adiciona-o à lista de 
-componentes a encomendar</t>
-  </si>
-  <si>
-    <t>3.2. Indica novo componente a 
-encomendar e a sua quantidade</t>
   </si>
   <si>
     <t>Funcionário</t>
@@ -350,9 +311,6 @@
     <t>4. Atualiza o stock atual</t>
   </si>
   <si>
-    <t xml:space="preserve">2.1. Regista componente ao sistema </t>
-  </si>
-  <si>
     <t>2.2. Adiciona componente ao sistema</t>
   </si>
   <si>
@@ -507,13 +465,80 @@
   </si>
   <si>
     <t>3.2 Sistema cancela a encomenda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1. Regista componente no sistema </t>
+  </si>
+  <si>
+    <t>1. Apresenta lista de stock</t>
+  </si>
+  <si>
+    <t>2.1. Não indica o componente</t>
+  </si>
+  <si>
+    <t>Cenário Alternativo 1
+[componente não existe no sistema]
+(passo 2)</t>
+  </si>
+  <si>
+    <t>2. Indica componente</t>
+  </si>
+  <si>
+    <t>2.1. Indica que componente não existe
+ no sistema</t>
+  </si>
+  <si>
+    <t>2.2. Pergunta se quer adicionar componente ao sistema</t>
+  </si>
+  <si>
+    <t>2.3. Aceita registar componente</t>
+  </si>
+  <si>
+    <t>2.4. Regista componente no sistema</t>
+  </si>
+  <si>
+    <t>2.5. Regressa a 3</t>
+  </si>
+  <si>
+    <t>3. Pergunta qual a quantidade a encomendar</t>
+  </si>
+  <si>
+    <t>4. Indica a quantidade</t>
+  </si>
+  <si>
+    <t>5. Encomenda o componente indicado</t>
+  </si>
+  <si>
+    <t>Cenário Exceção 2
+[não indica quantidades]
+(passo 4)</t>
+  </si>
+  <si>
+    <t>4.1. Não indica a quantidade</t>
+  </si>
+  <si>
+    <t>4.2. Informa que seleção foi cancelada</t>
+  </si>
+  <si>
+    <t>Cenário Exceção 3
+[não aceitar registar componente]
+(passo 2.3)</t>
+  </si>
+  <si>
+    <t>2.3.1. Não aceita registar componente</t>
+  </si>
+  <si>
+    <t>2.3.2. Informa que seleção foi cancelada</t>
+  </si>
+  <si>
+    <t>Componente encomendado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -576,7 +601,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -819,11 +844,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -905,9 +939,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -945,66 +976,68 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1319,52 +1352,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.125" customWidth="1"/>
+    <col min="3" max="3" width="33.375" customWidth="1"/>
     <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="2" spans="2:4" ht="19.5" thickBot="1">
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="49"/>
-    </row>
-    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="51"/>
+      <c r="D2" s="52"/>
+    </row>
+    <row r="3" spans="2:4" ht="19.5" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="49"/>
-    </row>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="51"/>
+      <c r="D3" s="52"/>
+    </row>
+    <row r="4" spans="2:4" ht="19.5" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="49"/>
-    </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="51"/>
+      <c r="D4" s="52"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="49"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="50" t="s">
+      <c r="C5" s="51"/>
+      <c r="D5" s="52"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B6" s="53" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1374,74 +1407,74 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="51"/>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B7" s="54"/>
       <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="51"/>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B8" s="54"/>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
+    <row r="9" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B9" s="54"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="51"/>
+    <row r="10" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B10" s="54"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="51"/>
+    <row r="11" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B11" s="54"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51"/>
+    <row r="12" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B12" s="54"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="51"/>
+    <row r="13" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B13" s="54"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="51"/>
+    <row r="14" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B14" s="54"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51"/>
+    <row r="15" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B15" s="54"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="51"/>
+    <row r="16" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B16" s="54"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="47" t="s">
+    <row r="17" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B17" s="50" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="47"/>
+    <row r="18" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B18" s="50"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="47"/>
+    <row r="19" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B19" s="50"/>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
     </row>
@@ -1459,59 +1492,59 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B3:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" customWidth="1"/>
+    <col min="3" max="3" width="32.625" customWidth="1"/>
+    <col min="4" max="4" width="34.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="4" spans="2:4" ht="19.5" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="49"/>
-    </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="52"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="49"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="52"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1">
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="49"/>
-    </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="52"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1">
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="49"/>
-    </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="50" t="s">
+      <c r="C7" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="52"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B8" s="53" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -1521,73 +1554,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
+    <row r="9" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B9" s="54"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="51"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B10" s="54"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="51"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B11" s="54"/>
       <c r="C11" s="12" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51"/>
+    <row r="12" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B12" s="54"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="51"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B13" s="54"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="51"/>
+    <row r="14" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B14" s="54"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51"/>
+    <row r="15" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B15" s="54"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="51"/>
+    <row r="16" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B16" s="54"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="51"/>
+    <row r="17" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B17" s="54"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" ht="38.25" thickBot="1">
       <c r="B18" s="65" t="s">
-        <v>113</v>
-      </c>
-      <c r="C18" s="64" t="s">
-        <v>111</v>
+        <v>101</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>99</v>
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="47"/>
+    <row r="19" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B19" s="50"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="36" t="s">
-        <v>112</v>
+      <c r="D19" s="35" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1604,67 +1637,67 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:F24"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:D24"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" customWidth="1"/>
-    <col min="4" max="4" width="66.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.875" customWidth="1"/>
+    <col min="3" max="3" width="40.625" customWidth="1"/>
+    <col min="4" max="4" width="66.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" ht="16.5" thickBot="1">
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
     </row>
-    <row r="2" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="19.5" thickBot="1">
       <c r="B2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="57"/>
+      <c r="D2" s="60"/>
       <c r="E2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="19.5" thickBot="1">
       <c r="B3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="57"/>
-    </row>
-    <row r="4" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="60"/>
+    </row>
+    <row r="4" spans="2:5" ht="19.5" thickBot="1">
       <c r="B4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="57"/>
-    </row>
-    <row r="5" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="60"/>
+    </row>
+    <row r="5" spans="2:5" ht="19.5" thickBot="1">
       <c r="B5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="57"/>
-    </row>
-    <row r="6" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="50" t="s">
+      <c r="D5" s="60"/>
+    </row>
+    <row r="6" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B6" s="53" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -1674,141 +1707,141 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="50"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="39" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="50"/>
-      <c r="C8" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="37"/>
-    </row>
-    <row r="9" spans="2:5" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="51"/>
+    <row r="7" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B7" s="53"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B8" s="53"/>
+      <c r="C8" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="36"/>
+    </row>
+    <row r="9" spans="2:5" ht="71.099999999999994" customHeight="1" thickBot="1">
+      <c r="B9" s="54"/>
       <c r="C9" s="18"/>
       <c r="D9" s="19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="58" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="51"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="57" thickBot="1">
+      <c r="B10" s="54"/>
       <c r="C10" s="18"/>
       <c r="D10" s="19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="51"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B11" s="54"/>
       <c r="C11" s="18"/>
       <c r="D11" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="58" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="51"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="57" thickBot="1">
+      <c r="B12" s="54"/>
       <c r="C12" s="18"/>
       <c r="D12" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="54" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="38.25" thickBot="1">
+      <c r="B13" s="57" t="s">
+        <v>23</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="47"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B14" s="50"/>
       <c r="C14" s="29" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D14" s="31"/>
     </row>
-    <row r="15" spans="2:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="47"/>
+    <row r="15" spans="2:5" ht="39.75" customHeight="1" thickBot="1">
+      <c r="B15" s="50"/>
       <c r="C15" s="28"/>
       <c r="D15" s="30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="55" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B16" s="58" t="s">
+        <v>24</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="19.5" thickBot="1">
+      <c r="B17" s="50"/>
       <c r="C17" s="18" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D17" s="19"/>
     </row>
-    <row r="18" spans="2:6" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="47"/>
+    <row r="18" spans="2:6" ht="51.75" customHeight="1" thickBot="1">
+      <c r="B18" s="50"/>
       <c r="C18" s="22"/>
       <c r="D18" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="52" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="39.950000000000003" customHeight="1">
+      <c r="B19" s="55" t="s">
+        <v>29</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D19" s="26"/>
     </row>
-    <row r="20" spans="2:6" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="53"/>
+    <row r="20" spans="2:6" ht="39.950000000000003" customHeight="1" thickBot="1">
+      <c r="B20" s="56"/>
       <c r="C20" s="27"/>
       <c r="D20" s="19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="54" t="s">
-        <v>41</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="38.1" customHeight="1" thickBot="1">
+      <c r="B21" s="57" t="s">
+        <v>30</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D21" s="26"/>
     </row>
-    <row r="22" spans="2:6" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="47"/>
+    <row r="22" spans="2:6" ht="39.950000000000003" customHeight="1" thickBot="1">
+      <c r="B22" s="50"/>
       <c r="C22" s="22"/>
       <c r="D22" s="24" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="2:6" ht="19" x14ac:dyDescent="0.2">
-      <c r="B23" s="52" t="s">
-        <v>49</v>
+    <row r="23" spans="2:6" ht="18.75">
+      <c r="B23" s="55" t="s">
+        <v>38</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D23" s="26"/>
     </row>
-    <row r="24" spans="2:6" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="53"/>
-      <c r="C24" s="41"/>
+    <row r="24" spans="2:6" ht="47.25" customHeight="1" thickBot="1">
+      <c r="B24" s="56"/>
+      <c r="C24" s="40"/>
       <c r="D24" s="24" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1830,59 +1863,59 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:D13"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" customWidth="1"/>
-    <col min="4" max="4" width="40.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.375" customWidth="1"/>
+    <col min="3" max="3" width="36.625" customWidth="1"/>
+    <col min="4" max="4" width="40.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="2" spans="2:4" ht="19.5" thickBot="1">
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="49"/>
-    </row>
-    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="52"/>
+    </row>
+    <row r="3" spans="2:4" ht="19.5" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="49"/>
-    </row>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="52"/>
+    </row>
+    <row r="4" spans="2:4" ht="19.5" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="60"/>
-    </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="63"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="49"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="50" t="s">
+      <c r="C5" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="52"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B6" s="53" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1892,55 +1925,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="51"/>
+    <row r="7" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B7" s="54"/>
       <c r="C7" s="12" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="51"/>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B8" s="54"/>
       <c r="C8" s="12"/>
       <c r="D8" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B9" s="54"/>
       <c r="C9" s="12" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="51"/>
+    <row r="10" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B10" s="54"/>
       <c r="C10" s="5"/>
       <c r="D10" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="54" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>83</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="38.25" customHeight="1" thickBot="1">
+      <c r="B11" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>117</v>
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="54"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="46" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="47"/>
+    <row r="12" spans="2:4" ht="38.25" customHeight="1" thickBot="1">
+      <c r="B12" s="57"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="56.25" customHeight="1" thickBot="1">
+      <c r="B13" s="50"/>
       <c r="C13" s="6"/>
       <c r="D13" s="24" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1958,55 +1991,59 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B1:D23"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" customWidth="1"/>
-    <col min="4" max="4" width="40.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.375" customWidth="1"/>
+    <col min="3" max="3" width="36.625" customWidth="1"/>
+    <col min="4" max="4" width="46.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="2" spans="2:4" ht="19.5" thickBot="1">
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="49"/>
-    </row>
-    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="52"/>
+    </row>
+    <row r="3" spans="2:4" ht="19.5" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="49"/>
-    </row>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="52"/>
+    </row>
+    <row r="4" spans="2:4" ht="19.5" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="49"/>
-    </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="52"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="49"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="50" t="s">
+      <c r="C5" s="62" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="52"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B6" s="53" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2016,107 +2053,140 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="50"/>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B7" s="53"/>
       <c r="C7" s="32"/>
       <c r="D7" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="58" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="51"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B8" s="54"/>
       <c r="C8" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="34"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B9" s="54"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B10" s="54"/>
+      <c r="C10" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="34"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B11" s="54"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B12" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="2:4" ht="85.5" customHeight="1" thickBot="1">
+      <c r="B13" s="50"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="35"/>
-    </row>
-    <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="51"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="33"/>
-    </row>
-    <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="54" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="47"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="47"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>22</v>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B14" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>131</v>
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="47"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="47"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="54" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="47"/>
-      <c r="C18" s="12" t="s">
-        <v>27</v>
+    <row r="15" spans="2:4" ht="84" customHeight="1" thickBot="1">
+      <c r="B15" s="50"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="35" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B16" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="33"/>
+      <c r="D16" s="41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B17" s="57"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B18" s="57"/>
+      <c r="C18" s="68" t="s">
+        <v>124</v>
       </c>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="2:4" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="47"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="36" t="s">
-        <v>26</v>
-      </c>
+    <row r="19" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B19" s="57"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="20.25" customHeight="1" thickBot="1">
+      <c r="B20" s="50"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B21" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="2:4" ht="78.75" customHeight="1" thickBot="1">
+      <c r="B22" s="50"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="D23" s="67"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B19"/>
+  <mergeCells count="9">
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B14:B15"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2124,60 +2194,60 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" customWidth="1"/>
-    <col min="4" max="4" width="53.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.625" customWidth="1"/>
+    <col min="3" max="3" width="33.375" customWidth="1"/>
+    <col min="4" max="4" width="53.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="2" spans="2:4" ht="19.5" thickBot="1">
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="49"/>
-    </row>
-    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="52"/>
+    </row>
+    <row r="3" spans="2:4" ht="19.5" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="49"/>
-    </row>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="52"/>
+    </row>
+    <row r="4" spans="2:4" ht="19.5" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="49"/>
-    </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="52"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="49"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="50" t="s">
+      <c r="C5" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="52"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B6" s="53" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2187,154 +2257,154 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="51"/>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B7" s="54"/>
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="51"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B8" s="54"/>
       <c r="C8" s="5" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
+    <row r="9" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B9" s="54"/>
       <c r="C9" s="5"/>
       <c r="D9" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="51"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B10" s="54"/>
       <c r="C10" s="5"/>
       <c r="D10" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="51"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B11" s="54"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="43" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51"/>
+      <c r="D11" s="42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B12" s="54"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="51"/>
+    <row r="13" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B13" s="54"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="51"/>
+    <row r="14" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B14" s="54"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51"/>
+    <row r="15" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B15" s="54"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="51"/>
+    <row r="16" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B16" s="54"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="54" t="s">
-        <v>59</v>
+    <row r="17" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B17" s="57" t="s">
+        <v>48</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="47"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B18" s="50"/>
       <c r="C18" s="12" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="47"/>
+    <row r="19" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B19" s="50"/>
       <c r="C19" s="12"/>
       <c r="D19" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="47"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B20" s="50"/>
       <c r="C20" s="12"/>
       <c r="D20" s="19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="47"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="24" customHeight="1" thickBot="1">
+      <c r="B21" s="50"/>
       <c r="C21" s="6"/>
       <c r="D21" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="54" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B22" s="57" t="s">
+        <v>49</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="42" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="47"/>
+      <c r="D22" s="41" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B23" s="50"/>
       <c r="C23" s="12" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="47"/>
+    <row r="24" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B24" s="50"/>
       <c r="C24" s="12"/>
       <c r="D24" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="47"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B25" s="50"/>
       <c r="C25" s="12"/>
       <c r="D25" s="19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="47"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="20.25" customHeight="1" thickBot="1">
+      <c r="B26" s="50"/>
       <c r="C26" s="6"/>
       <c r="D26" s="23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="B27" s="52" t="s">
-        <v>74</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="18.75">
+      <c r="B27" s="55" t="s">
+        <v>63</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D27" s="26"/>
     </row>
-    <row r="28" spans="2:4" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="53"/>
-      <c r="C28" s="41"/>
+    <row r="28" spans="2:4" ht="54" customHeight="1" thickBot="1">
+      <c r="B28" s="56"/>
+      <c r="C28" s="40"/>
       <c r="D28" s="24" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2353,59 +2423,59 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:D22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="B4:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.5" customWidth="1"/>
+    <col min="2" max="2" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="32.25" customWidth="1"/>
+    <col min="4" max="4" width="37.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" s="49"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="52"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1">
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="49"/>
-    </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="52"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1">
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="48" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7" s="49"/>
-    </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="52"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1">
       <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="48" t="s">
-        <v>121</v>
-      </c>
-      <c r="D8" s="49"/>
-    </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="50" t="s">
+      <c r="C8" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="52"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B9" s="53" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -2415,191 +2485,192 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="51"/>
+    <row r="10" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B10" s="54"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="51"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B11" s="54"/>
       <c r="C11" s="5"/>
       <c r="D11" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B12" s="54"/>
       <c r="C12" s="5" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="51"/>
+    <row r="13" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B13" s="54"/>
       <c r="C13" s="5"/>
       <c r="D13" s="10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="51"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B14" s="54"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B15" s="54"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="51"/>
+    <row r="16" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B16" s="54"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="51"/>
+    <row r="17" spans="2:7" ht="19.5" thickBot="1">
+      <c r="B17" s="54"/>
       <c r="C17" s="5"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="51"/>
+    <row r="18" spans="2:7" ht="19.5" thickBot="1">
+      <c r="B18" s="54"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="51"/>
+    <row r="19" spans="2:7" ht="19.5" thickBot="1">
+      <c r="B19" s="54"/>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="62" t="s">
-        <v>126</v>
-      </c>
-      <c r="C20" s="64" t="s">
-        <v>127</v>
+    <row r="20" spans="2:7" ht="19.5" thickBot="1">
+      <c r="B20" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" s="47" t="s">
+        <v>115</v>
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="47"/>
+    <row r="21" spans="2:7" ht="67.5" customHeight="1" thickBot="1">
+      <c r="B21" s="50"/>
       <c r="C21" s="5"/>
       <c r="D21" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="47"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="3"/>
+        <v>116</v>
+      </c>
+      <c r="G21" s="67"/>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="G22" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B9:B19"/>
-    <mergeCell ref="B20:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C4:E14"/>
   <sheetViews>
     <sheetView topLeftCell="B2" workbookViewId="0">
       <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="17.5" customWidth="1"/>
     <col min="4" max="4" width="29.5" customWidth="1"/>
-    <col min="5" max="5" width="37.33203125" customWidth="1"/>
+    <col min="5" max="5" width="37.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:5" ht="16.5" thickBot="1"/>
+    <row r="5" spans="3:5" ht="19.5" thickBot="1">
       <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="E5" s="49"/>
-    </row>
-    <row r="6" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="52"/>
+    </row>
+    <row r="6" spans="3:5" ht="19.5" thickBot="1">
       <c r="C6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="49"/>
-    </row>
-    <row r="7" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="52"/>
+    </row>
+    <row r="7" spans="3:5" ht="19.5" thickBot="1">
       <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="E7" s="49"/>
-    </row>
-    <row r="8" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="52"/>
+    </row>
+    <row r="8" spans="3:5" ht="19.5" thickBot="1">
       <c r="C8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="49"/>
-    </row>
-    <row r="9" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="50" t="s">
+      <c r="D8" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="52"/>
+    </row>
+    <row r="9" spans="3:5" ht="19.5" thickBot="1">
+      <c r="C9" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="66" t="s">
+      <c r="D9" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="67" t="s">
+      <c r="E9" s="49" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="51"/>
+    <row r="10" spans="3:5" ht="38.25" thickBot="1">
+      <c r="C10" s="54"/>
       <c r="D10" s="12" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="51"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" ht="19.5" thickBot="1">
+      <c r="C11" s="54"/>
       <c r="D11" s="5"/>
       <c r="E11" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="51"/>
-      <c r="D12" s="63"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" ht="19.5" thickBot="1">
+      <c r="C12" s="54"/>
+      <c r="D12" s="46"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="51"/>
+    <row r="13" spans="3:5" ht="19.5" thickBot="1">
+      <c r="C13" s="54"/>
       <c r="D13" s="5"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="51"/>
+    <row r="14" spans="3:5" ht="19.5" thickBot="1">
+      <c r="C14" s="54"/>
       <c r="D14" s="6"/>
       <c r="E14" s="3"/>
     </row>
@@ -2616,59 +2687,59 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B3:D24"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
     <col min="3" max="3" width="28.5" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="33.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="4" spans="2:4" ht="19.5" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="49"/>
-    </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="52"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="49"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="52"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1">
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="49"/>
-    </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="52"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1">
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="49"/>
-    </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="50" t="s">
+      <c r="C7" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="52"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B8" s="53" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -2678,101 +2749,101 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
+    <row r="9" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B9" s="54"/>
       <c r="C9" s="12" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="51"/>
+    <row r="10" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B10" s="54"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="51"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B11" s="54"/>
       <c r="C11" s="5"/>
       <c r="D11" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B12" s="54"/>
       <c r="C12" s="12" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="51"/>
+    <row r="13" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B13" s="54"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="51"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B14" s="54"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51"/>
+    <row r="15" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B15" s="54"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="51"/>
+    <row r="16" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B16" s="54"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="51"/>
+    <row r="17" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B17" s="54"/>
       <c r="C17" s="5"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="51"/>
+    <row r="18" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B18" s="54"/>
       <c r="C18" s="6"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="62" t="s">
-        <v>100</v>
+    <row r="19" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B19" s="64" t="s">
+        <v>88</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="47"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B20" s="50"/>
       <c r="C20" s="5"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="47"/>
+    <row r="21" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B21" s="50"/>
       <c r="C21" s="6"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="62" t="s">
-        <v>102</v>
+    <row r="22" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B22" s="64" t="s">
+        <v>90</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="42" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="47"/>
+      <c r="D22" s="41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B23" s="50"/>
       <c r="C23" s="5"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="47"/>
+    <row r="24" spans="2:4" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B24" s="50"/>
       <c r="C24" s="6"/>
       <c r="D24" s="3"/>
     </row>
@@ -2791,59 +2862,59 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B3:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
+    <col min="3" max="3" width="29.375" customWidth="1"/>
+    <col min="4" max="4" width="32.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="4" spans="2:4" ht="19.5" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="48" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="49"/>
-    </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="52"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="49"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="52"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1">
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="49"/>
-    </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="52"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1">
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="48" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7" s="49"/>
-    </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="50" t="s">
+      <c r="C7" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="52"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B8" s="53" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -2853,62 +2924,62 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
+    <row r="9" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B9" s="54"/>
       <c r="C9" s="5" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="51"/>
+    <row r="10" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B10" s="54"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="51"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B11" s="54"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51"/>
+    <row r="12" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B12" s="54"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="51"/>
+    <row r="13" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B13" s="54"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="62" t="s">
-        <v>107</v>
+    <row r="14" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B14" s="64" t="s">
+        <v>95</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="42" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="47"/>
+      <c r="D14" s="41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B15" s="50"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="47"/>
+    <row r="16" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B16" s="50"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="B8:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Use cases de fábrica prontos
</commit_message>
<xml_diff>
--- a/Use Cases.xlsx
+++ b/Use Cases.xlsx
@@ -9,24 +9,26 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11920" yWindow="460" windowWidth="13680" windowHeight="15540" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="11920" yWindow="460" windowWidth="13680" windowHeight="15540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Login" sheetId="19" r:id="rId2"/>
-    <sheet name="Adiciona Componente" sheetId="4" r:id="rId3"/>
-    <sheet name="Configuração Ótima" sheetId="18" r:id="rId4"/>
-    <sheet name="Registar Entrada Stock" sheetId="10" r:id="rId5"/>
-    <sheet name="Encomendar Stock" sheetId="11" r:id="rId6"/>
-    <sheet name="Adiciona Pacote" sheetId="12" r:id="rId7"/>
-    <sheet name="Regista Encomenda" sheetId="17" r:id="rId8"/>
-    <sheet name="Consultar cliente" sheetId="13" r:id="rId9"/>
-    <sheet name="Registar cliente" sheetId="14" r:id="rId10"/>
-    <sheet name="Identificar Cliente" sheetId="16" r:id="rId11"/>
-    <sheet name="Alterar Cliente" sheetId="15" r:id="rId12"/>
-    <sheet name="Registar Funcionário" sheetId="20" r:id="rId13"/>
-    <sheet name="Remover Funcionário" sheetId="21" r:id="rId14"/>
-    <sheet name="Alterar Funcionário" sheetId="22" r:id="rId15"/>
+    <sheet name="Processar Encomenda" sheetId="24" r:id="rId2"/>
+    <sheet name="Login" sheetId="19" r:id="rId3"/>
+    <sheet name="Adiciona Componente" sheetId="4" r:id="rId4"/>
+    <sheet name="Configuração Ótima" sheetId="18" r:id="rId5"/>
+    <sheet name="Registar Entrada Stock" sheetId="10" r:id="rId6"/>
+    <sheet name="Encomendar Stock" sheetId="11" r:id="rId7"/>
+    <sheet name="Adiciona Pacote" sheetId="12" r:id="rId8"/>
+    <sheet name="Regista Encomenda" sheetId="17" r:id="rId9"/>
+    <sheet name="Consultar encomenda" sheetId="23" r:id="rId10"/>
+    <sheet name="Consultar cliente" sheetId="13" r:id="rId11"/>
+    <sheet name="Registar cliente" sheetId="14" r:id="rId12"/>
+    <sheet name="Identificar Cliente" sheetId="16" r:id="rId13"/>
+    <sheet name="Alterar Cliente" sheetId="15" r:id="rId14"/>
+    <sheet name="Registar Funcionário" sheetId="20" r:id="rId15"/>
+    <sheet name="Remover Funcionário" sheetId="21" r:id="rId16"/>
+    <sheet name="Alterar Funcionário" sheetId="22" r:id="rId17"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="239">
   <si>
     <t>Actor input</t>
   </si>
@@ -824,6 +826,95 @@
   </si>
   <si>
     <t>1.2.2 Cancela a operação</t>
+  </si>
+  <si>
+    <t>Detalhes Encomenda</t>
+  </si>
+  <si>
+    <t>Gestor Fábrica</t>
+  </si>
+  <si>
+    <t>Gestor autenticado</t>
+  </si>
+  <si>
+    <t>1. Disponibiliza as encomendas em 
+queue</t>
+  </si>
+  <si>
+    <t>2. Seleciona a encomenda 
+desejada</t>
+  </si>
+  <si>
+    <t>3. Mostra os detalhes a encomenda
+ selecionada</t>
+  </si>
+  <si>
+    <t>Dados da encomenda disponibilizados</t>
+  </si>
+  <si>
+    <t>Cenário Exception 1
+ [Nenhuma encomenda selecionada]
+ (Passo 2)</t>
+  </si>
+  <si>
+    <t>2.1 Não seleciona uma 
+encomenda</t>
+  </si>
+  <si>
+    <t>2.2 Informa que o procedimento 
+foi cancelado</t>
+  </si>
+  <si>
+    <t>Produzir Encomenda</t>
+  </si>
+  <si>
+    <t>Encomenda processada</t>
+  </si>
+  <si>
+    <t>1. Disponibiliza as encomendas 
+da queue</t>
+  </si>
+  <si>
+    <t>2. Seleciona a encomenda 
+pretendida</t>
+  </si>
+  <si>
+    <t>3. Verifica se existe stock para 
+processa encomenda</t>
+  </si>
+  <si>
+    <t>4. Processa Encomenda</t>
+  </si>
+  <si>
+    <t>3.1 Informa o funcionário que não tem stock para processar a encomenda</t>
+  </si>
+  <si>
+    <t>Cenário Excepção 1 
+[Stock insuficiente] 
+(Passo 3)</t>
+  </si>
+  <si>
+    <t>Cenário Alternativo 1 
+[Não quer componentes] 
+(Passo 3)</t>
+  </si>
+  <si>
+    <t>3.2 Pergunta se quer lista com os componentes em falta</t>
+  </si>
+  <si>
+    <t>3.3 Indica a sua decisão</t>
+  </si>
+  <si>
+    <t>3.4 Apresenta lista</t>
+  </si>
+  <si>
+    <t>3.5 Cancela procedimento</t>
+  </si>
+  <si>
+    <t>3.3.1 Indica que não quer saber</t>
+  </si>
+  <si>
+    <t>Regressa para 3.5</t>
   </si>
 </sst>
 </file>
@@ -1286,6 +1377,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1333,9 +1427,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1670,32 +1761,32 @@
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="57"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="57"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="58" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1706,73 +1797,73 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="58"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="58"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="58"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="58"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="58"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="58"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="58"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="58"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="58"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="58"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="55" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="54"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="54"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
     </row>
@@ -1790,6 +1881,265 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:D22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="36.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>214</v>
+      </c>
+      <c r="D5" s="57"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>215</v>
+      </c>
+      <c r="D6" s="57"/>
+    </row>
+    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" s="57"/>
+    </row>
+    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>220</v>
+      </c>
+      <c r="D8" s="57"/>
+    </row>
+    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="59"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="59"/>
+      <c r="C11" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="59"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="59"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="59"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="59"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="59"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="59"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="59"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="59"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="60" t="s">
+        <v>221</v>
+      </c>
+      <c r="C20" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="55"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="10" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="55"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B9:B19"/>
+    <mergeCell ref="B20:B22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:E14"/>
+  <sheetViews>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
+    <col min="5" max="5" width="37.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="57"/>
+    </row>
+    <row r="6" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="57"/>
+    </row>
+    <row r="7" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="57"/>
+    </row>
+    <row r="8" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="57"/>
+    </row>
+    <row r="9" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="49" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="59"/>
+      <c r="D10" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="59"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="59"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="59"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="59"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C9:C14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D24"/>
   <sheetViews>
@@ -1809,40 +2159,40 @@
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="56"/>
+      <c r="D6" s="57"/>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="57"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -1853,67 +2203,67 @@
       </c>
     </row>
     <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="58"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="12" t="s">
         <v>76</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="58"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="58"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="5"/>
       <c r="D11" s="10" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="58"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="12" t="s">
         <v>79</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="58"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="58"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="58"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="58"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="58"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="5"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="58"/>
+      <c r="B18" s="59"/>
       <c r="C18" s="6"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="60" t="s">
         <v>81</v>
       </c>
       <c r="C19" s="4"/>
@@ -1922,17 +2272,17 @@
       </c>
     </row>
     <row r="20" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="54"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="5"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="54"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="6"/>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="60" t="s">
         <v>83</v>
       </c>
       <c r="C22" s="47" t="s">
@@ -1941,14 +2291,14 @@
       <c r="D22" s="41"/>
     </row>
     <row r="23" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="54"/>
+      <c r="B23" s="55"/>
       <c r="C23" s="5"/>
       <c r="D23" s="10" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="54"/>
+      <c r="B24" s="55"/>
       <c r="C24" s="6"/>
       <c r="D24" s="3"/>
     </row>
@@ -1966,7 +2316,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D16"/>
   <sheetViews>
@@ -1986,40 +2336,40 @@
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="56"/>
+      <c r="D6" s="57"/>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="57"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -2030,36 +2380,36 @@
       </c>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="58"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="5" t="s">
         <v>86</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="58"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="58"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="58"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="58"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="60" t="s">
         <v>87</v>
       </c>
       <c r="C14" s="4"/>
@@ -2068,12 +2418,12 @@
       </c>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="54"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="54"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
@@ -2090,7 +2440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D19"/>
   <sheetViews>
@@ -2110,40 +2460,40 @@
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="56"/>
+      <c r="D6" s="57"/>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="57"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -2154,60 +2504,60 @@
       </c>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="58"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="58"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="58"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="12" t="s">
         <v>93</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="58"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="58"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="58"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="58"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="58"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="58"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="69" t="s">
+      <c r="B18" s="70" t="s">
         <v>92</v>
       </c>
       <c r="C18" s="47" t="s">
@@ -2216,7 +2566,7 @@
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="54"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="6"/>
       <c r="D19" s="35" t="s">
         <v>91</v>
@@ -2235,7 +2585,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D27"/>
   <sheetViews>
@@ -2255,40 +2605,40 @@
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="56" t="s">
         <v>153</v>
       </c>
-      <c r="D6" s="56"/>
+      <c r="D6" s="57"/>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="56" t="s">
         <v>154</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="57"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -2299,67 +2649,67 @@
       </c>
     </row>
     <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="58"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="12" t="s">
         <v>156</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="58"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="58"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="5"/>
       <c r="D11" s="10" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="58"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="12" t="s">
         <v>158</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="58"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="58"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="58"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="58"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="58"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="5"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="58"/>
+      <c r="B18" s="59"/>
       <c r="C18" s="6"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="63" t="s">
         <v>160</v>
       </c>
       <c r="C19" s="47" t="s">
@@ -2368,21 +2718,21 @@
       <c r="D19" s="41"/>
     </row>
     <row r="20" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="62"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="5"/>
       <c r="D20" s="10" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="54"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="5"/>
       <c r="D21" s="1" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="62" t="s">
+      <c r="B22" s="63" t="s">
         <v>161</v>
       </c>
       <c r="C22" s="4"/>
@@ -2391,19 +2741,19 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="54"/>
+      <c r="B23" s="55"/>
       <c r="C23" s="5"/>
       <c r="D23" s="1" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="54"/>
+      <c r="B24" s="55"/>
       <c r="C24" s="6"/>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="62" t="s">
+      <c r="B25" s="63" t="s">
         <v>163</v>
       </c>
       <c r="C25" s="47" t="s">
@@ -2412,14 +2762,14 @@
       <c r="D25" s="41"/>
     </row>
     <row r="26" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="62"/>
+      <c r="B26" s="63"/>
       <c r="C26" s="5"/>
       <c r="D26" s="10" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="54"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="6"/>
       <c r="D27" s="3" t="s">
         <v>186</v>
@@ -2440,7 +2790,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D27"/>
   <sheetViews>
@@ -2460,40 +2810,40 @@
       <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>165</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="D6" s="56"/>
+      <c r="D6" s="57"/>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="56" t="s">
         <v>153</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="57"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="D8" s="56"/>
+      <c r="D8" s="57"/>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="58" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -2504,67 +2854,67 @@
       </c>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="58"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="5" t="s">
         <v>167</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="58"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="5"/>
       <c r="D11" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="58"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="5"/>
       <c r="D12" s="10" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="58"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="5" t="s">
         <v>170</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="58"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="58"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="58"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="58"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="5"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="58"/>
+      <c r="B18" s="59"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="58"/>
+      <c r="B19" s="59"/>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="60" t="s">
         <v>172</v>
       </c>
       <c r="C20" s="47" t="s">
@@ -2573,14 +2923,14 @@
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="54"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="5"/>
       <c r="D21" s="10" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="58" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="62" t="s">
+      <c r="B22" s="63" t="s">
         <v>189</v>
       </c>
       <c r="C22" s="4"/>
@@ -2589,17 +2939,17 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="54"/>
+      <c r="B23" s="55"/>
       <c r="C23" s="5"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="54"/>
+      <c r="B24" s="55"/>
       <c r="C24" s="6"/>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="62" t="s">
+      <c r="B25" s="63" t="s">
         <v>191</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -2608,14 +2958,14 @@
       <c r="D25" s="41"/>
     </row>
     <row r="26" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="54"/>
+      <c r="B26" s="55"/>
       <c r="C26" s="5"/>
       <c r="D26" s="10" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="54"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="6"/>
       <c r="D27" s="3"/>
     </row>
@@ -2634,7 +2984,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D24"/>
   <sheetViews>
@@ -2654,40 +3004,40 @@
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="56" t="s">
         <v>193</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="56" t="s">
         <v>153</v>
       </c>
-      <c r="D6" s="56"/>
+      <c r="D6" s="57"/>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="56" t="s">
         <v>194</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="57"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -2698,67 +3048,67 @@
       </c>
     </row>
     <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="58"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="12" t="s">
         <v>195</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="58"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="5"/>
       <c r="D10" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="58"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="5"/>
       <c r="D11" s="10" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="58"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="12" t="s">
         <v>198</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="58"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="58"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="58"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="58"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="58"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="5"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="58"/>
+      <c r="B18" s="59"/>
       <c r="C18" s="6"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="60" t="s">
         <v>172</v>
       </c>
       <c r="C19" s="47" t="s">
@@ -2767,14 +3117,14 @@
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="54"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="5"/>
       <c r="D20" s="10" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="58" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="63" t="s">
         <v>189</v>
       </c>
       <c r="C21" s="4"/>
@@ -2783,12 +3133,12 @@
       </c>
     </row>
     <row r="22" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="54"/>
+      <c r="B22" s="55"/>
       <c r="C22" s="6"/>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="69" t="s">
+      <c r="B23" s="70" t="s">
         <v>200</v>
       </c>
       <c r="C23" s="47" t="s">
@@ -2797,7 +3147,7 @@
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="54"/>
+      <c r="B24" s="55"/>
       <c r="C24" s="6"/>
       <c r="D24" s="35" t="s">
         <v>202</v>
@@ -2819,6 +3169,194 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" s="57"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="57"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>216</v>
+      </c>
+      <c r="D6" s="57"/>
+    </row>
+    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>225</v>
+      </c>
+      <c r="D7" s="57"/>
+    </row>
+    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="59"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="59"/>
+      <c r="C10" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="59"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="10" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="59"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="59"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="59"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="59"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="59"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="59"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="59"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="2:4" ht="58" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="63" t="s">
+        <v>231</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="41" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="63"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="63"/>
+      <c r="C21" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="63"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="10" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="55"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="60" t="s">
+        <v>232</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D24" s="41"/>
+    </row>
+    <row r="25" spans="2:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="55"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B8:B18"/>
+    <mergeCell ref="B19:B23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D20"/>
   <sheetViews>
@@ -2838,38 +3376,38 @@
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="57"/>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="57"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -2880,65 +3418,65 @@
       </c>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="58"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="58"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="12" t="s">
         <v>146</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="77" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="58"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="5"/>
       <c r="D11" s="53" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="58"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="5"/>
       <c r="D12" s="10" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="58"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="58"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="58"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="58"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="58"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="5"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="58"/>
+      <c r="B18" s="59"/>
       <c r="C18" s="6"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="60" t="s">
         <v>148</v>
       </c>
       <c r="C19" s="4"/>
@@ -2947,7 +3485,7 @@
       </c>
     </row>
     <row r="20" spans="2:4" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="54"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="6"/>
       <c r="D20" s="3"/>
     </row>
@@ -2964,7 +3502,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F24"/>
   <sheetViews>
@@ -2989,10 +3527,10 @@
       <c r="B2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="65"/>
+      <c r="D2" s="66"/>
       <c r="E2" s="11" t="s">
         <v>10</v>
       </c>
@@ -3001,31 +3539,31 @@
       <c r="B3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="65"/>
+      <c r="D3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="65"/>
+      <c r="D4" s="66"/>
     </row>
     <row r="5" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="65"/>
+      <c r="D5" s="66"/>
     </row>
     <row r="6" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="58" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -3036,49 +3574,49 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="57"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="37"/>
       <c r="D7" s="38" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="57"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="39" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="36"/>
     </row>
     <row r="9" spans="2:5" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="58"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="18"/>
       <c r="D9" s="19" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="58" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="58"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="18"/>
       <c r="D10" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="58"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="18"/>
       <c r="D11" s="19" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="58" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="58"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="18"/>
       <c r="D12" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="62" t="s">
+      <c r="B13" s="63" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="20"/>
@@ -3087,21 +3625,21 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="54"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="29" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="31"/>
     </row>
     <row r="15" spans="2:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="54"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="28"/>
       <c r="D15" s="30" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="64" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="18"/>
@@ -3110,21 +3648,21 @@
       </c>
     </row>
     <row r="17" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="54"/>
+      <c r="B17" s="55"/>
       <c r="C17" s="18" t="s">
         <v>28</v>
       </c>
       <c r="D17" s="19"/>
     </row>
     <row r="18" spans="2:6" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="54"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="22"/>
       <c r="D18" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="61" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="25" t="s">
@@ -3133,14 +3671,14 @@
       <c r="D19" s="26"/>
     </row>
     <row r="20" spans="2:6" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="61"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="27"/>
       <c r="D20" s="19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="63" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="25" t="s">
@@ -3149,7 +3687,7 @@
       <c r="D21" s="26"/>
     </row>
     <row r="22" spans="2:6" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="54"/>
+      <c r="B22" s="55"/>
       <c r="C22" s="22"/>
       <c r="D22" s="24" t="s">
         <v>37</v>
@@ -3157,7 +3695,7 @@
       <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" ht="19" x14ac:dyDescent="0.2">
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="61" t="s">
         <v>38</v>
       </c>
       <c r="C23" s="25" t="s">
@@ -3166,7 +3704,7 @@
       <c r="D23" s="26"/>
     </row>
     <row r="24" spans="2:6" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="61"/>
+      <c r="B24" s="62"/>
       <c r="C24" s="40"/>
       <c r="D24" s="24" t="s">
         <v>40</v>
@@ -3190,7 +3728,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D29"/>
   <sheetViews>
@@ -3210,40 +3748,40 @@
       <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="56"/>
+      <c r="D6" s="57"/>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="57"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="D8" s="56"/>
+      <c r="D8" s="57"/>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="58" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -3254,73 +3792,73 @@
       </c>
     </row>
     <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="58"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="5"/>
       <c r="D10" s="10" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="58"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="12" t="s">
         <v>130</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="58"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="5"/>
       <c r="D12" s="10" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="58"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="12" t="s">
         <v>132</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="58"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="58" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="58"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="5"/>
       <c r="D15" s="10" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="58"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="5" t="s">
         <v>135</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="58"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="5"/>
       <c r="D17" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="58"/>
+      <c r="B18" s="59"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="58"/>
+      <c r="B19" s="59"/>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="60" t="s">
         <v>137</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -3329,19 +3867,19 @@
       <c r="D20" s="41"/>
     </row>
     <row r="21" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="54"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="5"/>
       <c r="D21" s="10" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="54"/>
+      <c r="B22" s="55"/>
       <c r="C22" s="6"/>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="60" t="s">
         <v>139</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -3350,14 +3888,14 @@
       <c r="D23" s="41"/>
     </row>
     <row r="24" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="54"/>
+      <c r="B24" s="55"/>
       <c r="C24" s="6"/>
       <c r="D24" s="35" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="60" t="s">
         <v>177</v>
       </c>
       <c r="C25" s="47" t="s">
@@ -3366,14 +3904,14 @@
       <c r="D25" s="41"/>
     </row>
     <row r="26" spans="2:4" ht="47" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="54"/>
+      <c r="B26" s="55"/>
       <c r="C26" s="6"/>
       <c r="D26" s="35" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="60" t="s">
         <v>138</v>
       </c>
       <c r="C27" s="47" t="s">
@@ -3384,14 +3922,14 @@
       </c>
     </row>
     <row r="28" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="59"/>
+      <c r="B28" s="60"/>
       <c r="C28" s="12"/>
       <c r="D28" s="10" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="54"/>
+      <c r="B29" s="55"/>
       <c r="C29" s="6"/>
       <c r="D29" s="35" t="s">
         <v>35</v>
@@ -3413,11 +3951,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -3433,40 +3971,40 @@
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="56"/>
+      <c r="D2" s="57"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="57"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="69"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="58" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -3477,33 +4015,33 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="58"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="12" t="s">
         <v>203</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="58"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="12" t="s">
         <v>206</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="58"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="12"/>
       <c r="D9" s="1" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="58"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="5"/>
       <c r="D10" s="10"/>
     </row>
     <row r="11" spans="2:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="63" t="s">
         <v>204</v>
       </c>
       <c r="C11" s="43" t="s">
@@ -3512,28 +4050,28 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="2:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="62"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="44"/>
       <c r="D12" s="10" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="62"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="44"/>
       <c r="D13" s="45" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="54"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="6"/>
       <c r="D14" s="24" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="60" t="s">
         <v>211</v>
       </c>
       <c r="C15" s="43"/>
@@ -3542,15 +4080,15 @@
       </c>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="62"/>
+      <c r="B16" s="63"/>
       <c r="C16" s="44"/>
       <c r="D16" s="10" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="62"/>
-      <c r="C17" s="70"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="54"/>
       <c r="D17" s="23"/>
     </row>
   </sheetData>
@@ -3568,7 +4106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D23"/>
   <sheetViews>
@@ -3588,40 +4126,40 @@
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="56"/>
+      <c r="D2" s="57"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="57"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="68" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="58" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -3632,42 +4170,42 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="57"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="32"/>
       <c r="D7" s="13" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="58"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="12" t="s">
         <v>111</v>
       </c>
       <c r="D8" s="34"/>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="58"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="12"/>
       <c r="D9" s="34" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="58"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="12" t="s">
         <v>118</v>
       </c>
       <c r="D10" s="34"/>
     </row>
     <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="58"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="5"/>
       <c r="D11" s="10" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="62" t="s">
+      <c r="B12" s="63" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="33" t="s">
@@ -3676,14 +4214,14 @@
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="2:4" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="54"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="5"/>
       <c r="D13" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="63" t="s">
         <v>120</v>
       </c>
       <c r="C14" s="33" t="s">
@@ -3692,14 +4230,14 @@
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="2:4" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="54"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="6"/>
       <c r="D15" s="35" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="63" t="s">
         <v>110</v>
       </c>
       <c r="C16" s="33"/>
@@ -3708,35 +4246,35 @@
       </c>
     </row>
     <row r="17" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="62"/>
+      <c r="B17" s="63"/>
       <c r="C17" s="52"/>
       <c r="D17" s="10" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="62"/>
+      <c r="B18" s="63"/>
       <c r="C18" s="52" t="s">
         <v>114</v>
       </c>
       <c r="D18" s="10"/>
     </row>
     <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="62"/>
+      <c r="B19" s="63"/>
       <c r="C19" s="52"/>
       <c r="D19" s="10" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="54"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="6"/>
       <c r="D20" s="35" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="63" t="s">
         <v>123</v>
       </c>
       <c r="C21" s="33" t="s">
@@ -3745,7 +4283,7 @@
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="2:4" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="54"/>
+      <c r="B22" s="55"/>
       <c r="C22" s="6"/>
       <c r="D22" s="35" t="s">
         <v>125</v>
@@ -3771,7 +4309,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D28"/>
   <sheetViews>
@@ -3792,40 +4330,40 @@
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="56"/>
+      <c r="D2" s="57"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="57"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="58" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -3836,67 +4374,67 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="58"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="58"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="58"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="5"/>
       <c r="D9" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="58"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="5"/>
       <c r="D10" s="10" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="58"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="5"/>
       <c r="D11" s="42" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="58"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="58"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="58"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="58"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="58"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="63" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="4"/>
@@ -3905,35 +4443,35 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="54"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="12" t="s">
         <v>51</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="54"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="12"/>
       <c r="D19" s="10" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="54"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="12"/>
       <c r="D20" s="19" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="54"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="6"/>
       <c r="D21" s="23" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="62" t="s">
+      <c r="B22" s="63" t="s">
         <v>49</v>
       </c>
       <c r="C22" s="4"/>
@@ -3942,35 +4480,35 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="54"/>
+      <c r="B23" s="55"/>
       <c r="C23" s="12" t="s">
         <v>54</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="54"/>
+      <c r="B24" s="55"/>
       <c r="C24" s="12"/>
       <c r="D24" s="10" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="54"/>
+      <c r="B25" s="55"/>
       <c r="C25" s="12"/>
       <c r="D25" s="19" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="54"/>
+      <c r="B26" s="55"/>
       <c r="C26" s="6"/>
       <c r="D26" s="23" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="B27" s="60" t="s">
+      <c r="B27" s="61" t="s">
         <v>63</v>
       </c>
       <c r="C27" s="25" t="s">
@@ -3979,7 +4517,7 @@
       <c r="D27" s="26"/>
     </row>
     <row r="28" spans="2:4" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="61"/>
+      <c r="B28" s="62"/>
       <c r="C28" s="40"/>
       <c r="D28" s="24" t="s">
         <v>62</v>
@@ -4000,7 +4538,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G22"/>
   <sheetViews>
@@ -4020,40 +4558,40 @@
       <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="56"/>
+      <c r="D6" s="57"/>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="57"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="56"/>
+      <c r="D8" s="57"/>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="58" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -4064,67 +4602,67 @@
       </c>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="58"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="58"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="5"/>
       <c r="D11" s="10" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="58"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="5" t="s">
         <v>102</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="58"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="5"/>
       <c r="D13" s="10" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="58"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="58"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="58"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="58"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="5"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="58"/>
+      <c r="B18" s="59"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="58"/>
+      <c r="B19" s="59"/>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="2:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="60" t="s">
         <v>105</v>
       </c>
       <c r="C20" s="47" t="s">
@@ -4133,7 +4671,7 @@
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="2:7" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="54"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="5"/>
       <c r="D21" s="1" t="s">
         <v>107</v>
@@ -4156,110 +4694,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:E14"/>
-  <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="29.5" customWidth="1"/>
-    <col min="5" max="5" width="37.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="3:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="56"/>
-    </row>
-    <row r="6" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="56"/>
-    </row>
-    <row r="7" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="55" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="56"/>
-    </row>
-    <row r="8" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="56"/>
-    </row>
-    <row r="9" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="49" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="58"/>
-      <c r="D10" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="58"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="58"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="58"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="58"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C9:C14"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>